<commit_message>
Added script to classify protein seq into BCR/TCR/MHC chains.
</commit_message>
<xml_diff>
--- a/out/MRO_HMM_out.xlsx
+++ b/out/MRO_HMM_out.xlsx
@@ -12,18 +12,18 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25425" windowHeight="10380"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="DTU_MHC-I" sheetId="2" r:id="rId2"/>
     <sheet name="Pfam_MHC-I" sheetId="5" r:id="rId3"/>
     <sheet name="Pfam_MHC-II_alpha" sheetId="3" r:id="rId4"/>
     <sheet name="Pfam_MHC-II_beta" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$E$387</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DTU_MHC-I'!$A$1:$B$218</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pfam_MHC-I'!$A$1:$B$211</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Pfam_MHC-II_alpha'!$A$1:$B$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Pfam_MHC-II_beta'!$A$1:$B$131</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$387</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>LEN($E2)</f>
+        <f t="shared" ref="D2:D65" si="0">LEN($E2)</f>
         <v>353</v>
       </c>
       <c r="E2" t="s">
@@ -2717,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>LEN($E3)</f>
+        <f t="shared" si="0"/>
         <v>361</v>
       </c>
       <c r="E3" t="s">
@@ -2735,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f>LEN($E4)</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="E4" t="s">
@@ -2753,7 +2753,7 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <f>LEN($E5)</f>
+        <f t="shared" si="0"/>
         <v>358</v>
       </c>
       <c r="E5" t="s">
@@ -2771,7 +2771,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <f>LEN($E6)</f>
+        <f t="shared" si="0"/>
         <v>361</v>
       </c>
       <c r="E6" t="s">
@@ -2789,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <f>LEN($E7)</f>
+        <f t="shared" si="0"/>
         <v>355</v>
       </c>
       <c r="E7" t="s">
@@ -2807,7 +2807,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <f>LEN($E8)</f>
+        <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="E8" t="s">
@@ -2825,7 +2825,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <f>LEN($E9)</f>
+        <f t="shared" si="0"/>
         <v>355</v>
       </c>
       <c r="E9" t="s">
@@ -2843,7 +2843,7 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <f>LEN($E10)</f>
+        <f t="shared" si="0"/>
         <v>358</v>
       </c>
       <c r="E10" t="s">
@@ -2861,7 +2861,7 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <f>LEN($E11)</f>
+        <f t="shared" si="0"/>
         <v>358</v>
       </c>
       <c r="E11" t="s">
@@ -2873,7 +2873,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <f>LEN($E12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2888,7 +2888,7 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <f>LEN($E13)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="E13" t="s">
@@ -2906,7 +2906,7 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <f>LEN($E14)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="E14" t="s">
@@ -2924,7 +2924,7 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <f>LEN($E15)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="E15" t="s">
@@ -2942,7 +2942,7 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <f>LEN($E16)</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="E16" t="s">
@@ -2960,7 +2960,7 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <f>LEN($E17)</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="E17" t="s">
@@ -2978,7 +2978,7 @@
         <v>13</v>
       </c>
       <c r="D18">
-        <f>LEN($E18)</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="E18" t="s">
@@ -2996,7 +2996,7 @@
         <v>13</v>
       </c>
       <c r="D19">
-        <f>LEN($E19)</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="E19" t="s">
@@ -3008,7 +3008,7 @@
         <v>14</v>
       </c>
       <c r="D20">
-        <f>LEN($E20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <f>LEN($E21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3032,7 +3032,7 @@
         <v>17</v>
       </c>
       <c r="D22">
-        <f>LEN($E22)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="E22" t="s">
@@ -3050,7 +3050,7 @@
         <v>18</v>
       </c>
       <c r="D23">
-        <f>LEN($E23)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="E23" t="s">
@@ -3068,7 +3068,7 @@
         <v>22</v>
       </c>
       <c r="D24">
-        <f>LEN($E24)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="E24" t="s">
@@ -3086,7 +3086,7 @@
         <v>23</v>
       </c>
       <c r="D25">
-        <f>LEN($E25)</f>
+        <f t="shared" si="0"/>
         <v>261</v>
       </c>
       <c r="E25" t="s">
@@ -3104,7 +3104,7 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <f>LEN($E26)</f>
+        <f t="shared" si="0"/>
         <v>261</v>
       </c>
       <c r="E26" t="s">
@@ -3122,7 +3122,7 @@
         <v>20</v>
       </c>
       <c r="D27">
-        <f>LEN($E27)</f>
+        <f t="shared" si="0"/>
         <v>261</v>
       </c>
       <c r="E27" t="s">
@@ -3140,7 +3140,7 @@
         <v>20</v>
       </c>
       <c r="D28">
-        <f>LEN($E28)</f>
+        <f t="shared" si="0"/>
         <v>261</v>
       </c>
       <c r="E28" t="s">
@@ -3158,7 +3158,7 @@
         <v>21</v>
       </c>
       <c r="D29">
-        <f>LEN($E29)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="E29" t="s">
@@ -3176,7 +3176,7 @@
         <v>24</v>
       </c>
       <c r="D30">
-        <f>LEN($E30)</f>
+        <f t="shared" si="0"/>
         <v>221</v>
       </c>
       <c r="E30" t="s">
@@ -3188,7 +3188,7 @@
         <v>25</v>
       </c>
       <c r="D31">
-        <f>LEN($E31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3203,7 +3203,7 @@
         <v>26</v>
       </c>
       <c r="D32">
-        <f>LEN($E32)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E32" t="s">
@@ -3221,7 +3221,7 @@
         <v>27</v>
       </c>
       <c r="D33">
-        <f>LEN($E33)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E33" t="s">
@@ -3239,7 +3239,7 @@
         <v>28</v>
       </c>
       <c r="D34">
-        <f>LEN($E34)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E34" t="s">
@@ -3257,7 +3257,7 @@
         <v>29</v>
       </c>
       <c r="D35">
-        <f>LEN($E35)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="E35" t="s">
@@ -3275,7 +3275,7 @@
         <v>36</v>
       </c>
       <c r="D36">
-        <f>LEN($E36)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E36" t="s">
@@ -3287,7 +3287,7 @@
         <v>30</v>
       </c>
       <c r="D37">
-        <f>LEN($E37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3302,7 +3302,7 @@
         <v>31</v>
       </c>
       <c r="D38">
-        <f>LEN($E38)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="E38" t="s">
@@ -3320,7 +3320,7 @@
         <v>32</v>
       </c>
       <c r="D39">
-        <f>LEN($E39)</f>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="E39" t="s">
@@ -3338,7 +3338,7 @@
         <v>33</v>
       </c>
       <c r="D40">
-        <f>LEN($E40)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E40" t="s">
@@ -3356,7 +3356,7 @@
         <v>34</v>
       </c>
       <c r="D41">
-        <f>LEN($E41)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="E41" t="s">
@@ -3374,7 +3374,7 @@
         <v>35</v>
       </c>
       <c r="D42">
-        <f>LEN($E42)</f>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="E42" t="s">
@@ -3386,7 +3386,7 @@
         <v>372</v>
       </c>
       <c r="D43">
-        <f>LEN($E43)</f>
+        <f t="shared" si="0"/>
         <v>333</v>
       </c>
       <c r="E43" t="s">
@@ -3398,7 +3398,7 @@
         <v>373</v>
       </c>
       <c r="D44">
-        <f>LEN($E44)</f>
+        <f t="shared" si="0"/>
         <v>445</v>
       </c>
       <c r="E44" t="s">
@@ -3416,7 +3416,7 @@
         <v>374</v>
       </c>
       <c r="D45">
-        <f>LEN($E45)</f>
+        <f t="shared" si="0"/>
         <v>336</v>
       </c>
       <c r="E45" t="s">
@@ -3434,7 +3434,7 @@
         <v>37</v>
       </c>
       <c r="D46">
-        <f>LEN($E46)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
       <c r="E46" t="s">
@@ -3452,7 +3452,7 @@
         <v>38</v>
       </c>
       <c r="D47">
-        <f>LEN($E47)</f>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
       <c r="E47" t="s">
@@ -3470,7 +3470,7 @@
         <v>39</v>
       </c>
       <c r="D48">
-        <f>LEN($E48)</f>
+        <f t="shared" si="0"/>
         <v>277</v>
       </c>
       <c r="E48" t="s">
@@ -3488,7 +3488,7 @@
         <v>40</v>
       </c>
       <c r="D49">
-        <f>LEN($E49)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E49" t="s">
@@ -3506,7 +3506,7 @@
         <v>41</v>
       </c>
       <c r="D50">
-        <f>LEN($E50)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E50" t="s">
@@ -3524,7 +3524,7 @@
         <v>42</v>
       </c>
       <c r="D51">
-        <f>LEN($E51)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E51" t="s">
@@ -3542,7 +3542,7 @@
         <v>43</v>
       </c>
       <c r="D52">
-        <f>LEN($E52)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E52" t="s">
@@ -3560,7 +3560,7 @@
         <v>44</v>
       </c>
       <c r="D53">
-        <f>LEN($E53)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E53" t="s">
@@ -3578,7 +3578,7 @@
         <v>45</v>
       </c>
       <c r="D54">
-        <f>LEN($E54)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E54" t="s">
@@ -3596,7 +3596,7 @@
         <v>46</v>
       </c>
       <c r="D55">
-        <f>LEN($E55)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E55" t="s">
@@ -3614,7 +3614,7 @@
         <v>47</v>
       </c>
       <c r="D56">
-        <f>LEN($E56)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E56" t="s">
@@ -3632,7 +3632,7 @@
         <v>48</v>
       </c>
       <c r="D57">
-        <f>LEN($E57)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E57" t="s">
@@ -3650,7 +3650,7 @@
         <v>49</v>
       </c>
       <c r="D58">
-        <f>LEN($E58)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E58" t="s">
@@ -3668,7 +3668,7 @@
         <v>50</v>
       </c>
       <c r="D59">
-        <f>LEN($E59)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E59" t="s">
@@ -3686,7 +3686,7 @@
         <v>51</v>
       </c>
       <c r="D60">
-        <f>LEN($E60)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E60" t="s">
@@ -3704,7 +3704,7 @@
         <v>52</v>
       </c>
       <c r="D61">
-        <f>LEN($E61)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E61" t="s">
@@ -3722,7 +3722,7 @@
         <v>53</v>
       </c>
       <c r="D62">
-        <f>LEN($E62)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E62" t="s">
@@ -3740,7 +3740,7 @@
         <v>54</v>
       </c>
       <c r="D63">
-        <f>LEN($E63)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E63" t="s">
@@ -3758,7 +3758,7 @@
         <v>55</v>
       </c>
       <c r="D64">
-        <f>LEN($E64)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E64" t="s">
@@ -3776,7 +3776,7 @@
         <v>56</v>
       </c>
       <c r="D65">
-        <f>LEN($E65)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="E65" t="s">
@@ -3794,7 +3794,7 @@
         <v>57</v>
       </c>
       <c r="D66">
-        <f>LEN($E66)</f>
+        <f t="shared" ref="D66:D129" si="1">LEN($E66)</f>
         <v>365</v>
       </c>
       <c r="E66" t="s">
@@ -3812,7 +3812,7 @@
         <v>58</v>
       </c>
       <c r="D67">
-        <f>LEN($E67)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E67" t="s">
@@ -3830,7 +3830,7 @@
         <v>59</v>
       </c>
       <c r="D68">
-        <f>LEN($E68)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E68" t="s">
@@ -3848,7 +3848,7 @@
         <v>60</v>
       </c>
       <c r="D69">
-        <f>LEN($E69)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E69" t="s">
@@ -3866,7 +3866,7 @@
         <v>61</v>
       </c>
       <c r="D70">
-        <f>LEN($E70)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E70" t="s">
@@ -3884,7 +3884,7 @@
         <v>62</v>
       </c>
       <c r="D71">
-        <f>LEN($E71)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E71" t="s">
@@ -3902,7 +3902,7 @@
         <v>63</v>
       </c>
       <c r="D72">
-        <f>LEN($E72)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E72" t="s">
@@ -3920,7 +3920,7 @@
         <v>64</v>
       </c>
       <c r="D73">
-        <f>LEN($E73)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E73" t="s">
@@ -3938,7 +3938,7 @@
         <v>65</v>
       </c>
       <c r="D74">
-        <f>LEN($E74)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E74" t="s">
@@ -3956,7 +3956,7 @@
         <v>66</v>
       </c>
       <c r="D75">
-        <f>LEN($E75)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E75" t="s">
@@ -3974,7 +3974,7 @@
         <v>67</v>
       </c>
       <c r="D76">
-        <f>LEN($E76)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E76" t="s">
@@ -3992,7 +3992,7 @@
         <v>68</v>
       </c>
       <c r="D77">
-        <f>LEN($E77)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E77" t="s">
@@ -4010,7 +4010,7 @@
         <v>69</v>
       </c>
       <c r="D78">
-        <f>LEN($E78)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E78" t="s">
@@ -4028,7 +4028,7 @@
         <v>70</v>
       </c>
       <c r="D79">
-        <f>LEN($E79)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E79" t="s">
@@ -4046,7 +4046,7 @@
         <v>71</v>
       </c>
       <c r="D80">
-        <f>LEN($E80)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E80" t="s">
@@ -4064,7 +4064,7 @@
         <v>72</v>
       </c>
       <c r="D81">
-        <f>LEN($E81)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E81" t="s">
@@ -4082,7 +4082,7 @@
         <v>73</v>
       </c>
       <c r="D82">
-        <f>LEN($E82)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E82" t="s">
@@ -4100,7 +4100,7 @@
         <v>74</v>
       </c>
       <c r="D83">
-        <f>LEN($E83)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E83" t="s">
@@ -4118,7 +4118,7 @@
         <v>75</v>
       </c>
       <c r="D84">
-        <f>LEN($E84)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E84" t="s">
@@ -4136,7 +4136,7 @@
         <v>76</v>
       </c>
       <c r="D85">
-        <f>LEN($E85)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E85" t="s">
@@ -4154,7 +4154,7 @@
         <v>77</v>
       </c>
       <c r="D86">
-        <f>LEN($E86)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E86" t="s">
@@ -4172,7 +4172,7 @@
         <v>78</v>
       </c>
       <c r="D87">
-        <f>LEN($E87)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E87" t="s">
@@ -4190,7 +4190,7 @@
         <v>79</v>
       </c>
       <c r="D88">
-        <f>LEN($E88)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E88" t="s">
@@ -4208,7 +4208,7 @@
         <v>80</v>
       </c>
       <c r="D89">
-        <f>LEN($E89)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E89" t="s">
@@ -4226,7 +4226,7 @@
         <v>81</v>
       </c>
       <c r="D90">
-        <f>LEN($E90)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E90" t="s">
@@ -4244,7 +4244,7 @@
         <v>82</v>
       </c>
       <c r="D91">
-        <f>LEN($E91)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E91" t="s">
@@ -4262,7 +4262,7 @@
         <v>83</v>
       </c>
       <c r="D92">
-        <f>LEN($E92)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E92" t="s">
@@ -4280,7 +4280,7 @@
         <v>84</v>
       </c>
       <c r="D93">
-        <f>LEN($E93)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E93" t="s">
@@ -4298,7 +4298,7 @@
         <v>85</v>
       </c>
       <c r="D94">
-        <f>LEN($E94)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E94" t="s">
@@ -4316,7 +4316,7 @@
         <v>86</v>
       </c>
       <c r="D95">
-        <f>LEN($E95)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E95" t="s">
@@ -4334,7 +4334,7 @@
         <v>87</v>
       </c>
       <c r="D96">
-        <f>LEN($E96)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E96" t="s">
@@ -4352,7 +4352,7 @@
         <v>88</v>
       </c>
       <c r="D97">
-        <f>LEN($E97)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E97" t="s">
@@ -4370,7 +4370,7 @@
         <v>89</v>
       </c>
       <c r="D98">
-        <f>LEN($E98)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E98" t="s">
@@ -4388,7 +4388,7 @@
         <v>90</v>
       </c>
       <c r="D99">
-        <f>LEN($E99)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E99" t="s">
@@ -4406,7 +4406,7 @@
         <v>91</v>
       </c>
       <c r="D100">
-        <f>LEN($E100)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E100" t="s">
@@ -4424,7 +4424,7 @@
         <v>92</v>
       </c>
       <c r="D101">
-        <f>LEN($E101)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E101" t="s">
@@ -4442,7 +4442,7 @@
         <v>93</v>
       </c>
       <c r="D102">
-        <f>LEN($E102)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E102" t="s">
@@ -4460,7 +4460,7 @@
         <v>94</v>
       </c>
       <c r="D103">
-        <f>LEN($E103)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E103" t="s">
@@ -4478,7 +4478,7 @@
         <v>95</v>
       </c>
       <c r="D104">
-        <f>LEN($E104)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E104" t="s">
@@ -4496,7 +4496,7 @@
         <v>96</v>
       </c>
       <c r="D105">
-        <f>LEN($E105)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E105" t="s">
@@ -4514,7 +4514,7 @@
         <v>97</v>
       </c>
       <c r="D106">
-        <f>LEN($E106)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E106" t="s">
@@ -4532,7 +4532,7 @@
         <v>98</v>
       </c>
       <c r="D107">
-        <f>LEN($E107)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E107" t="s">
@@ -4550,7 +4550,7 @@
         <v>99</v>
       </c>
       <c r="D108">
-        <f>LEN($E108)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E108" t="s">
@@ -4568,7 +4568,7 @@
         <v>100</v>
       </c>
       <c r="D109">
-        <f>LEN($E109)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E109" t="s">
@@ -4586,7 +4586,7 @@
         <v>101</v>
       </c>
       <c r="D110">
-        <f>LEN($E110)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E110" t="s">
@@ -4604,7 +4604,7 @@
         <v>102</v>
       </c>
       <c r="D111">
-        <f>LEN($E111)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E111" t="s">
@@ -4622,7 +4622,7 @@
         <v>103</v>
       </c>
       <c r="D112">
-        <f>LEN($E112)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E112" t="s">
@@ -4640,7 +4640,7 @@
         <v>104</v>
       </c>
       <c r="D113">
-        <f>LEN($E113)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E113" t="s">
@@ -4658,7 +4658,7 @@
         <v>105</v>
       </c>
       <c r="D114">
-        <f>LEN($E114)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E114" t="s">
@@ -4676,7 +4676,7 @@
         <v>106</v>
       </c>
       <c r="D115">
-        <f>LEN($E115)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E115" t="s">
@@ -4694,7 +4694,7 @@
         <v>107</v>
       </c>
       <c r="D116">
-        <f>LEN($E116)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E116" t="s">
@@ -4712,7 +4712,7 @@
         <v>108</v>
       </c>
       <c r="D117">
-        <f>LEN($E117)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E117" t="s">
@@ -4730,7 +4730,7 @@
         <v>109</v>
       </c>
       <c r="D118">
-        <f>LEN($E118)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E118" t="s">
@@ -4748,7 +4748,7 @@
         <v>110</v>
       </c>
       <c r="D119">
-        <f>LEN($E119)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E119" t="s">
@@ -4766,7 +4766,7 @@
         <v>111</v>
       </c>
       <c r="D120">
-        <f>LEN($E120)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E120" t="s">
@@ -4784,7 +4784,7 @@
         <v>112</v>
       </c>
       <c r="D121">
-        <f>LEN($E121)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E121" t="s">
@@ -4802,7 +4802,7 @@
         <v>113</v>
       </c>
       <c r="D122">
-        <f>LEN($E122)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E122" t="s">
@@ -4820,7 +4820,7 @@
         <v>114</v>
       </c>
       <c r="D123">
-        <f>LEN($E123)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E123" t="s">
@@ -4838,7 +4838,7 @@
         <v>115</v>
       </c>
       <c r="D124">
-        <f>LEN($E124)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E124" t="s">
@@ -4856,7 +4856,7 @@
         <v>116</v>
       </c>
       <c r="D125">
-        <f>LEN($E125)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E125" t="s">
@@ -4874,7 +4874,7 @@
         <v>117</v>
       </c>
       <c r="D126">
-        <f>LEN($E126)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E126" t="s">
@@ -4892,7 +4892,7 @@
         <v>118</v>
       </c>
       <c r="D127">
-        <f>LEN($E127)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E127" t="s">
@@ -4910,7 +4910,7 @@
         <v>119</v>
       </c>
       <c r="D128">
-        <f>LEN($E128)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E128" t="s">
@@ -4928,7 +4928,7 @@
         <v>120</v>
       </c>
       <c r="D129">
-        <f>LEN($E129)</f>
+        <f t="shared" si="1"/>
         <v>362</v>
       </c>
       <c r="E129" t="s">
@@ -4946,7 +4946,7 @@
         <v>121</v>
       </c>
       <c r="D130">
-        <f>LEN($E130)</f>
+        <f t="shared" ref="D130:D193" si="2">LEN($E130)</f>
         <v>362</v>
       </c>
       <c r="E130" t="s">
@@ -4964,7 +4964,7 @@
         <v>122</v>
       </c>
       <c r="D131">
-        <f>LEN($E131)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E131" t="s">
@@ -4982,7 +4982,7 @@
         <v>123</v>
       </c>
       <c r="D132">
-        <f>LEN($E132)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E132" t="s">
@@ -5000,7 +5000,7 @@
         <v>124</v>
       </c>
       <c r="D133">
-        <f>LEN($E133)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E133" t="s">
@@ -5018,7 +5018,7 @@
         <v>125</v>
       </c>
       <c r="D134">
-        <f>LEN($E134)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E134" t="s">
@@ -5036,7 +5036,7 @@
         <v>126</v>
       </c>
       <c r="D135">
-        <f>LEN($E135)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E135" t="s">
@@ -5054,7 +5054,7 @@
         <v>127</v>
       </c>
       <c r="D136">
-        <f>LEN($E136)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E136" t="s">
@@ -5072,7 +5072,7 @@
         <v>128</v>
       </c>
       <c r="D137">
-        <f>LEN($E137)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E137" t="s">
@@ -5090,7 +5090,7 @@
         <v>129</v>
       </c>
       <c r="D138">
-        <f>LEN($E138)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E138" t="s">
@@ -5108,7 +5108,7 @@
         <v>130</v>
       </c>
       <c r="D139">
-        <f>LEN($E139)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E139" t="s">
@@ -5126,7 +5126,7 @@
         <v>131</v>
       </c>
       <c r="D140">
-        <f>LEN($E140)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E140" t="s">
@@ -5144,7 +5144,7 @@
         <v>132</v>
       </c>
       <c r="D141">
-        <f>LEN($E141)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E141" t="s">
@@ -5162,7 +5162,7 @@
         <v>133</v>
       </c>
       <c r="D142">
-        <f>LEN($E142)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E142" t="s">
@@ -5180,7 +5180,7 @@
         <v>134</v>
       </c>
       <c r="D143">
-        <f>LEN($E143)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E143" t="s">
@@ -5198,7 +5198,7 @@
         <v>135</v>
       </c>
       <c r="D144">
-        <f>LEN($E144)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E144" t="s">
@@ -5216,7 +5216,7 @@
         <v>136</v>
       </c>
       <c r="D145">
-        <f>LEN($E145)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E145" t="s">
@@ -5234,7 +5234,7 @@
         <v>137</v>
       </c>
       <c r="D146">
-        <f>LEN($E146)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E146" t="s">
@@ -5252,7 +5252,7 @@
         <v>138</v>
       </c>
       <c r="D147">
-        <f>LEN($E147)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E147" t="s">
@@ -5270,7 +5270,7 @@
         <v>139</v>
       </c>
       <c r="D148">
-        <f>LEN($E148)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E148" t="s">
@@ -5288,7 +5288,7 @@
         <v>140</v>
       </c>
       <c r="D149">
-        <f>LEN($E149)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E149" t="s">
@@ -5306,7 +5306,7 @@
         <v>141</v>
       </c>
       <c r="D150">
-        <f>LEN($E150)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E150" t="s">
@@ -5324,7 +5324,7 @@
         <v>142</v>
       </c>
       <c r="D151">
-        <f>LEN($E151)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E151" t="s">
@@ -5342,7 +5342,7 @@
         <v>143</v>
       </c>
       <c r="D152">
-        <f>LEN($E152)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E152" t="s">
@@ -5360,7 +5360,7 @@
         <v>144</v>
       </c>
       <c r="D153">
-        <f>LEN($E153)</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="E153" t="s">
@@ -5378,7 +5378,7 @@
         <v>145</v>
       </c>
       <c r="D154">
-        <f>LEN($E154)</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="E154" t="s">
@@ -5396,7 +5396,7 @@
         <v>146</v>
       </c>
       <c r="D155">
-        <f>LEN($E155)</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="E155" t="s">
@@ -5414,7 +5414,7 @@
         <v>147</v>
       </c>
       <c r="D156">
-        <f>LEN($E156)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E156" t="s">
@@ -5432,7 +5432,7 @@
         <v>148</v>
       </c>
       <c r="D157">
-        <f>LEN($E157)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E157" t="s">
@@ -5450,7 +5450,7 @@
         <v>149</v>
       </c>
       <c r="D158">
-        <f>LEN($E158)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E158" t="s">
@@ -5468,7 +5468,7 @@
         <v>150</v>
       </c>
       <c r="D159">
-        <f>LEN($E159)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E159" t="s">
@@ -5486,7 +5486,7 @@
         <v>151</v>
       </c>
       <c r="D160">
-        <f>LEN($E160)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E160" t="s">
@@ -5504,7 +5504,7 @@
         <v>152</v>
       </c>
       <c r="D161">
-        <f>LEN($E161)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E161" t="s">
@@ -5522,7 +5522,7 @@
         <v>153</v>
       </c>
       <c r="D162">
-        <f>LEN($E162)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E162" t="s">
@@ -5540,7 +5540,7 @@
         <v>154</v>
       </c>
       <c r="D163">
-        <f>LEN($E163)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E163" t="s">
@@ -5558,7 +5558,7 @@
         <v>155</v>
       </c>
       <c r="D164">
-        <f>LEN($E164)</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="E164" t="s">
@@ -5576,7 +5576,7 @@
         <v>156</v>
       </c>
       <c r="D165">
-        <f>LEN($E165)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E165" t="s">
@@ -5594,7 +5594,7 @@
         <v>157</v>
       </c>
       <c r="D166">
-        <f>LEN($E166)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E166" t="s">
@@ -5612,7 +5612,7 @@
         <v>158</v>
       </c>
       <c r="D167">
-        <f>LEN($E167)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E167" t="s">
@@ -5630,7 +5630,7 @@
         <v>159</v>
       </c>
       <c r="D168">
-        <f>LEN($E168)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E168" t="s">
@@ -5648,7 +5648,7 @@
         <v>160</v>
       </c>
       <c r="D169">
-        <f>LEN($E169)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E169" t="s">
@@ -5666,7 +5666,7 @@
         <v>161</v>
       </c>
       <c r="D170">
-        <f>LEN($E170)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E170" t="s">
@@ -5684,7 +5684,7 @@
         <v>162</v>
       </c>
       <c r="D171">
-        <f>LEN($E171)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E171" t="s">
@@ -5702,7 +5702,7 @@
         <v>163</v>
       </c>
       <c r="D172">
-        <f>LEN($E172)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E172" t="s">
@@ -5720,7 +5720,7 @@
         <v>164</v>
       </c>
       <c r="D173">
-        <f>LEN($E173)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E173" t="s">
@@ -5738,7 +5738,7 @@
         <v>165</v>
       </c>
       <c r="D174">
-        <f>LEN($E174)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E174" t="s">
@@ -5756,7 +5756,7 @@
         <v>166</v>
       </c>
       <c r="D175">
-        <f>LEN($E175)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E175" t="s">
@@ -5774,7 +5774,7 @@
         <v>167</v>
       </c>
       <c r="D176">
-        <f>LEN($E176)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E176" t="s">
@@ -5792,7 +5792,7 @@
         <v>168</v>
       </c>
       <c r="D177">
-        <f>LEN($E177)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E177" t="s">
@@ -5810,7 +5810,7 @@
         <v>169</v>
       </c>
       <c r="D178">
-        <f>LEN($E178)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E178" t="s">
@@ -5828,7 +5828,7 @@
         <v>170</v>
       </c>
       <c r="D179">
-        <f>LEN($E179)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E179" t="s">
@@ -5846,7 +5846,7 @@
         <v>171</v>
       </c>
       <c r="D180">
-        <f>LEN($E180)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E180" t="s">
@@ -5864,7 +5864,7 @@
         <v>172</v>
       </c>
       <c r="D181">
-        <f>LEN($E181)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E181" t="s">
@@ -5882,7 +5882,7 @@
         <v>173</v>
       </c>
       <c r="D182">
-        <f>LEN($E182)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E182" t="s">
@@ -5900,7 +5900,7 @@
         <v>174</v>
       </c>
       <c r="D183">
-        <f>LEN($E183)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E183" t="s">
@@ -5918,7 +5918,7 @@
         <v>175</v>
       </c>
       <c r="D184">
-        <f>LEN($E184)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E184" t="s">
@@ -5936,7 +5936,7 @@
         <v>176</v>
       </c>
       <c r="D185">
-        <f>LEN($E185)</f>
+        <f t="shared" si="2"/>
         <v>363</v>
       </c>
       <c r="E185" t="s">
@@ -5954,7 +5954,7 @@
         <v>177</v>
       </c>
       <c r="D186">
-        <f>LEN($E186)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E186" t="s">
@@ -5972,7 +5972,7 @@
         <v>178</v>
       </c>
       <c r="D187">
-        <f>LEN($E187)</f>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="E187" t="s">
@@ -5990,7 +5990,7 @@
         <v>179</v>
       </c>
       <c r="D188">
-        <f>LEN($E188)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E188" t="s">
@@ -6008,7 +6008,7 @@
         <v>180</v>
       </c>
       <c r="D189">
-        <f>LEN($E189)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E189" t="s">
@@ -6026,7 +6026,7 @@
         <v>181</v>
       </c>
       <c r="D190">
-        <f>LEN($E190)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E190" t="s">
@@ -6044,7 +6044,7 @@
         <v>182</v>
       </c>
       <c r="D191">
-        <f>LEN($E191)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E191" t="s">
@@ -6062,7 +6062,7 @@
         <v>183</v>
       </c>
       <c r="D192">
-        <f>LEN($E192)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E192" t="s">
@@ -6080,7 +6080,7 @@
         <v>184</v>
       </c>
       <c r="D193">
-        <f>LEN($E193)</f>
+        <f t="shared" si="2"/>
         <v>366</v>
       </c>
       <c r="E193" t="s">
@@ -6098,7 +6098,7 @@
         <v>185</v>
       </c>
       <c r="D194">
-        <f>LEN($E194)</f>
+        <f t="shared" ref="D194:D257" si="3">LEN($E194)</f>
         <v>366</v>
       </c>
       <c r="E194" t="s">
@@ -6116,7 +6116,7 @@
         <v>186</v>
       </c>
       <c r="D195">
-        <f>LEN($E195)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E195" t="s">
@@ -6134,7 +6134,7 @@
         <v>187</v>
       </c>
       <c r="D196">
-        <f>LEN($E196)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E196" t="s">
@@ -6152,7 +6152,7 @@
         <v>188</v>
       </c>
       <c r="D197">
-        <f>LEN($E197)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E197" t="s">
@@ -6170,7 +6170,7 @@
         <v>189</v>
       </c>
       <c r="D198">
-        <f>LEN($E198)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E198" t="s">
@@ -6188,7 +6188,7 @@
         <v>190</v>
       </c>
       <c r="D199">
-        <f>LEN($E199)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E199" t="s">
@@ -6206,7 +6206,7 @@
         <v>191</v>
       </c>
       <c r="D200">
-        <f>LEN($E200)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E200" t="s">
@@ -6224,7 +6224,7 @@
         <v>192</v>
       </c>
       <c r="D201">
-        <f>LEN($E201)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E201" t="s">
@@ -6242,7 +6242,7 @@
         <v>193</v>
       </c>
       <c r="D202">
-        <f>LEN($E202)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E202" t="s">
@@ -6260,7 +6260,7 @@
         <v>194</v>
       </c>
       <c r="D203">
-        <f>LEN($E203)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E203" t="s">
@@ -6278,7 +6278,7 @@
         <v>195</v>
       </c>
       <c r="D204">
-        <f>LEN($E204)</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="E204" t="s">
@@ -6296,7 +6296,7 @@
         <v>196</v>
       </c>
       <c r="D205">
-        <f>LEN($E205)</f>
+        <f t="shared" si="3"/>
         <v>372</v>
       </c>
       <c r="E205" t="s">
@@ -6314,7 +6314,7 @@
         <v>197</v>
       </c>
       <c r="D206">
-        <f>LEN($E206)</f>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
       <c r="E206" t="s">
@@ -6332,7 +6332,7 @@
         <v>198</v>
       </c>
       <c r="D207">
-        <f>LEN($E207)</f>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
       <c r="E207" t="s">
@@ -6350,7 +6350,7 @@
         <v>199</v>
       </c>
       <c r="D208">
-        <f>LEN($E208)</f>
+        <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="E208" t="s">
@@ -6368,7 +6368,7 @@
         <v>200</v>
       </c>
       <c r="D209">
-        <f>LEN($E209)</f>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
       <c r="E209" t="s">
@@ -6386,7 +6386,7 @@
         <v>201</v>
       </c>
       <c r="D210">
-        <f>LEN($E210)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E210" t="s">
@@ -6404,7 +6404,7 @@
         <v>202</v>
       </c>
       <c r="D211">
-        <f>LEN($E211)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E211" t="s">
@@ -6422,7 +6422,7 @@
         <v>203</v>
       </c>
       <c r="D212">
-        <f>LEN($E212)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E212" t="s">
@@ -6440,7 +6440,7 @@
         <v>204</v>
       </c>
       <c r="D213">
-        <f>LEN($E213)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E213" t="s">
@@ -6458,7 +6458,7 @@
         <v>205</v>
       </c>
       <c r="D214">
-        <f>LEN($E214)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E214" t="s">
@@ -6476,7 +6476,7 @@
         <v>206</v>
       </c>
       <c r="D215">
-        <f>LEN($E215)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E215" t="s">
@@ -6494,7 +6494,7 @@
         <v>207</v>
       </c>
       <c r="D216">
-        <f>LEN($E216)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E216" t="s">
@@ -6512,7 +6512,7 @@
         <v>208</v>
       </c>
       <c r="D217">
-        <f>LEN($E217)</f>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="E217" t="s">
@@ -6530,7 +6530,7 @@
         <v>209</v>
       </c>
       <c r="D218">
-        <f>LEN($E218)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E218" t="s">
@@ -6548,7 +6548,7 @@
         <v>210</v>
       </c>
       <c r="D219">
-        <f>LEN($E219)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E219" t="s">
@@ -6566,7 +6566,7 @@
         <v>211</v>
       </c>
       <c r="D220">
-        <f>LEN($E220)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E220" t="s">
@@ -6584,7 +6584,7 @@
         <v>212</v>
       </c>
       <c r="D221">
-        <f>LEN($E221)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E221" t="s">
@@ -6602,7 +6602,7 @@
         <v>213</v>
       </c>
       <c r="D222">
-        <f>LEN($E222)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E222" t="s">
@@ -6620,7 +6620,7 @@
         <v>214</v>
       </c>
       <c r="D223">
-        <f>LEN($E223)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E223" t="s">
@@ -6638,7 +6638,7 @@
         <v>215</v>
       </c>
       <c r="D224">
-        <f>LEN($E224)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E224" t="s">
@@ -6656,7 +6656,7 @@
         <v>216</v>
       </c>
       <c r="D225">
-        <f>LEN($E225)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E225" t="s">
@@ -6674,7 +6674,7 @@
         <v>217</v>
       </c>
       <c r="D226">
-        <f>LEN($E226)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E226" t="s">
@@ -6692,7 +6692,7 @@
         <v>218</v>
       </c>
       <c r="D227">
-        <f>LEN($E227)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E227" t="s">
@@ -6710,7 +6710,7 @@
         <v>219</v>
       </c>
       <c r="D228">
-        <f>LEN($E228)</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="E228" t="s">
@@ -6728,7 +6728,7 @@
         <v>220</v>
       </c>
       <c r="D229">
-        <f>LEN($E229)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E229" t="s">
@@ -6746,7 +6746,7 @@
         <v>221</v>
       </c>
       <c r="D230">
-        <f>LEN($E230)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E230" t="s">
@@ -6764,7 +6764,7 @@
         <v>222</v>
       </c>
       <c r="D231">
-        <f>LEN($E231)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E231" t="s">
@@ -6782,7 +6782,7 @@
         <v>223</v>
       </c>
       <c r="D232">
-        <f>LEN($E232)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E232" t="s">
@@ -6800,7 +6800,7 @@
         <v>224</v>
       </c>
       <c r="D233">
-        <f>LEN($E233)</f>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="E233" t="s">
@@ -6818,7 +6818,7 @@
         <v>225</v>
       </c>
       <c r="D234">
-        <f>LEN($E234)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E234" t="s">
@@ -6836,7 +6836,7 @@
         <v>226</v>
       </c>
       <c r="D235">
-        <f>LEN($E235)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E235" t="s">
@@ -6854,7 +6854,7 @@
         <v>227</v>
       </c>
       <c r="D236">
-        <f>LEN($E236)</f>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="E236" t="s">
@@ -6872,7 +6872,7 @@
         <v>228</v>
       </c>
       <c r="D237">
-        <f>LEN($E237)</f>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="E237" t="s">
@@ -6890,7 +6890,7 @@
         <v>229</v>
       </c>
       <c r="D238">
-        <f>LEN($E238)</f>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="E238" t="s">
@@ -6908,7 +6908,7 @@
         <v>230</v>
       </c>
       <c r="D239">
-        <f>LEN($E239)</f>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="E239" t="s">
@@ -6926,7 +6926,7 @@
         <v>231</v>
       </c>
       <c r="D240">
-        <f>LEN($E240)</f>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="E240" t="s">
@@ -6944,7 +6944,7 @@
         <v>232</v>
       </c>
       <c r="D241">
-        <f>LEN($E241)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E241" t="s">
@@ -6962,7 +6962,7 @@
         <v>233</v>
       </c>
       <c r="D242">
-        <f>LEN($E242)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E242" t="s">
@@ -6980,7 +6980,7 @@
         <v>234</v>
       </c>
       <c r="D243">
-        <f>LEN($E243)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E243" t="s">
@@ -6998,7 +6998,7 @@
         <v>235</v>
       </c>
       <c r="D244">
-        <f>LEN($E244)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E244" t="s">
@@ -7016,7 +7016,7 @@
         <v>236</v>
       </c>
       <c r="D245">
-        <f>LEN($E245)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E245" t="s">
@@ -7034,7 +7034,7 @@
         <v>237</v>
       </c>
       <c r="D246">
-        <f>LEN($E246)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E246" t="s">
@@ -7052,7 +7052,7 @@
         <v>238</v>
       </c>
       <c r="D247">
-        <f>LEN($E247)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E247" t="s">
@@ -7070,7 +7070,7 @@
         <v>239</v>
       </c>
       <c r="D248">
-        <f>LEN($E248)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E248" t="s">
@@ -7088,7 +7088,7 @@
         <v>240</v>
       </c>
       <c r="D249">
-        <f>LEN($E249)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E249" t="s">
@@ -7106,7 +7106,7 @@
         <v>241</v>
       </c>
       <c r="D250">
-        <f>LEN($E250)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E250" t="s">
@@ -7124,7 +7124,7 @@
         <v>242</v>
       </c>
       <c r="D251">
-        <f>LEN($E251)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E251" t="s">
@@ -7142,7 +7142,7 @@
         <v>243</v>
       </c>
       <c r="D252">
-        <f>LEN($E252)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E252" t="s">
@@ -7160,7 +7160,7 @@
         <v>244</v>
       </c>
       <c r="D253">
-        <f>LEN($E253)</f>
+        <f t="shared" si="3"/>
         <v>269</v>
       </c>
       <c r="E253" t="s">
@@ -7178,7 +7178,7 @@
         <v>245</v>
       </c>
       <c r="D254">
-        <f>LEN($E254)</f>
+        <f t="shared" si="3"/>
         <v>269</v>
       </c>
       <c r="E254" t="s">
@@ -7196,7 +7196,7 @@
         <v>246</v>
       </c>
       <c r="D255">
-        <f>LEN($E255)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E255" t="s">
@@ -7214,7 +7214,7 @@
         <v>247</v>
       </c>
       <c r="D256">
-        <f>LEN($E256)</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="E256" t="s">
@@ -7232,7 +7232,7 @@
         <v>248</v>
       </c>
       <c r="D257">
-        <f>LEN($E257)</f>
+        <f t="shared" si="3"/>
         <v>277</v>
       </c>
       <c r="E257" t="s">
@@ -7250,7 +7250,7 @@
         <v>249</v>
       </c>
       <c r="D258">
-        <f>LEN($E258)</f>
+        <f t="shared" ref="D258:D321" si="4">LEN($E258)</f>
         <v>250</v>
       </c>
       <c r="E258" t="s">
@@ -7268,7 +7268,7 @@
         <v>250</v>
       </c>
       <c r="D259">
-        <f>LEN($E259)</f>
+        <f t="shared" si="4"/>
         <v>261</v>
       </c>
       <c r="E259" t="s">
@@ -7286,7 +7286,7 @@
         <v>251</v>
       </c>
       <c r="D260">
-        <f>LEN($E260)</f>
+        <f t="shared" si="4"/>
         <v>254</v>
       </c>
       <c r="E260" t="s">
@@ -7304,7 +7304,7 @@
         <v>252</v>
       </c>
       <c r="D261">
-        <f>LEN($E261)</f>
+        <f t="shared" si="4"/>
         <v>226</v>
       </c>
       <c r="E261" t="s">
@@ -7322,7 +7322,7 @@
         <v>253</v>
       </c>
       <c r="D262">
-        <f>LEN($E262)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E262" t="s">
@@ -7340,7 +7340,7 @@
         <v>254</v>
       </c>
       <c r="D263">
-        <f>LEN($E263)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E263" t="s">
@@ -7358,7 +7358,7 @@
         <v>255</v>
       </c>
       <c r="D264">
-        <f>LEN($E264)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E264" t="s">
@@ -7376,7 +7376,7 @@
         <v>256</v>
       </c>
       <c r="D265">
-        <f>LEN($E265)</f>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
       <c r="E265" t="s">
@@ -7394,7 +7394,7 @@
         <v>257</v>
       </c>
       <c r="D266">
-        <f>LEN($E266)</f>
+        <f t="shared" si="4"/>
         <v>183</v>
       </c>
       <c r="E266" t="s">
@@ -7412,7 +7412,7 @@
         <v>258</v>
       </c>
       <c r="D267">
-        <f>LEN($E267)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E267" t="s">
@@ -7430,7 +7430,7 @@
         <v>259</v>
       </c>
       <c r="D268">
-        <f>LEN($E268)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E268" t="s">
@@ -7448,7 +7448,7 @@
         <v>260</v>
       </c>
       <c r="D269">
-        <f>LEN($E269)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E269" t="s">
@@ -7466,7 +7466,7 @@
         <v>261</v>
       </c>
       <c r="D270">
-        <f>LEN($E270)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E270" t="s">
@@ -7484,7 +7484,7 @@
         <v>262</v>
       </c>
       <c r="D271">
-        <f>LEN($E271)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E271" t="s">
@@ -7502,7 +7502,7 @@
         <v>263</v>
       </c>
       <c r="D272">
-        <f>LEN($E272)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E272" t="s">
@@ -7520,7 +7520,7 @@
         <v>264</v>
       </c>
       <c r="D273">
-        <f>LEN($E273)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E273" t="s">
@@ -7538,7 +7538,7 @@
         <v>265</v>
       </c>
       <c r="D274">
-        <f>LEN($E274)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E274" t="s">
@@ -7556,7 +7556,7 @@
         <v>266</v>
       </c>
       <c r="D275">
-        <f>LEN($E275)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E275" t="s">
@@ -7574,7 +7574,7 @@
         <v>267</v>
       </c>
       <c r="D276">
-        <f>LEN($E276)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E276" t="s">
@@ -7592,7 +7592,7 @@
         <v>268</v>
       </c>
       <c r="D277">
-        <f>LEN($E277)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E277" t="s">
@@ -7610,7 +7610,7 @@
         <v>269</v>
       </c>
       <c r="D278">
-        <f>LEN($E278)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E278" t="s">
@@ -7628,7 +7628,7 @@
         <v>270</v>
       </c>
       <c r="D279">
-        <f>LEN($E279)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E279" t="s">
@@ -7646,7 +7646,7 @@
         <v>271</v>
       </c>
       <c r="D280">
-        <f>LEN($E280)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E280" t="s">
@@ -7664,7 +7664,7 @@
         <v>272</v>
       </c>
       <c r="D281">
-        <f>LEN($E281)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E281" t="s">
@@ -7682,7 +7682,7 @@
         <v>273</v>
       </c>
       <c r="D282">
-        <f>LEN($E282)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E282" t="s">
@@ -7700,7 +7700,7 @@
         <v>274</v>
       </c>
       <c r="D283">
-        <f>LEN($E283)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E283" t="s">
@@ -7718,7 +7718,7 @@
         <v>275</v>
       </c>
       <c r="D284">
-        <f>LEN($E284)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E284" t="s">
@@ -7736,7 +7736,7 @@
         <v>276</v>
       </c>
       <c r="D285">
-        <f>LEN($E285)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E285" t="s">
@@ -7754,7 +7754,7 @@
         <v>277</v>
       </c>
       <c r="D286">
-        <f>LEN($E286)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E286" t="s">
@@ -7772,7 +7772,7 @@
         <v>278</v>
       </c>
       <c r="D287">
-        <f>LEN($E287)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E287" t="s">
@@ -7790,7 +7790,7 @@
         <v>279</v>
       </c>
       <c r="D288">
-        <f>LEN($E288)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E288" t="s">
@@ -7808,7 +7808,7 @@
         <v>280</v>
       </c>
       <c r="D289">
-        <f>LEN($E289)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E289" t="s">
@@ -7826,7 +7826,7 @@
         <v>281</v>
       </c>
       <c r="D290">
-        <f>LEN($E290)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E290" t="s">
@@ -7844,7 +7844,7 @@
         <v>282</v>
       </c>
       <c r="D291">
-        <f>LEN($E291)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E291" t="s">
@@ -7862,7 +7862,7 @@
         <v>283</v>
       </c>
       <c r="D292">
-        <f>LEN($E292)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E292" t="s">
@@ -7880,7 +7880,7 @@
         <v>284</v>
       </c>
       <c r="D293">
-        <f>LEN($E293)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E293" t="s">
@@ -7898,7 +7898,7 @@
         <v>285</v>
       </c>
       <c r="D294">
-        <f>LEN($E294)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E294" t="s">
@@ -7916,7 +7916,7 @@
         <v>286</v>
       </c>
       <c r="D295">
-        <f>LEN($E295)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E295" t="s">
@@ -7934,7 +7934,7 @@
         <v>287</v>
       </c>
       <c r="D296">
-        <f>LEN($E296)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E296" t="s">
@@ -7952,7 +7952,7 @@
         <v>288</v>
       </c>
       <c r="D297">
-        <f>LEN($E297)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E297" t="s">
@@ -7970,7 +7970,7 @@
         <v>289</v>
       </c>
       <c r="D298">
-        <f>LEN($E298)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E298" t="s">
@@ -7988,7 +7988,7 @@
         <v>290</v>
       </c>
       <c r="D299">
-        <f>LEN($E299)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E299" t="s">
@@ -8006,7 +8006,7 @@
         <v>291</v>
       </c>
       <c r="D300">
-        <f>LEN($E300)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E300" t="s">
@@ -8024,7 +8024,7 @@
         <v>292</v>
       </c>
       <c r="D301">
-        <f>LEN($E301)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E301" t="s">
@@ -8042,7 +8042,7 @@
         <v>293</v>
       </c>
       <c r="D302">
-        <f>LEN($E302)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E302" t="s">
@@ -8060,7 +8060,7 @@
         <v>294</v>
       </c>
       <c r="D303">
-        <f>LEN($E303)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E303" t="s">
@@ -8078,7 +8078,7 @@
         <v>295</v>
       </c>
       <c r="D304">
-        <f>LEN($E304)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E304" t="s">
@@ -8096,7 +8096,7 @@
         <v>296</v>
       </c>
       <c r="D305">
-        <f>LEN($E305)</f>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="E305" t="s">
@@ -8114,7 +8114,7 @@
         <v>297</v>
       </c>
       <c r="D306">
-        <f>LEN($E306)</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E306" t="s">
@@ -8132,7 +8132,7 @@
         <v>298</v>
       </c>
       <c r="D307">
-        <f>LEN($E307)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E307" t="s">
@@ -8150,7 +8150,7 @@
         <v>299</v>
       </c>
       <c r="D308">
-        <f>LEN($E308)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E308" t="s">
@@ -8168,7 +8168,7 @@
         <v>300</v>
       </c>
       <c r="D309">
-        <f>LEN($E309)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E309" t="s">
@@ -8186,7 +8186,7 @@
         <v>301</v>
       </c>
       <c r="D310">
-        <f>LEN($E310)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E310" t="s">
@@ -8204,7 +8204,7 @@
         <v>302</v>
       </c>
       <c r="D311">
-        <f>LEN($E311)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E311" t="s">
@@ -8222,7 +8222,7 @@
         <v>303</v>
       </c>
       <c r="D312">
-        <f>LEN($E312)</f>
+        <f t="shared" si="4"/>
         <v>262</v>
       </c>
       <c r="E312" t="s">
@@ -8240,7 +8240,7 @@
         <v>304</v>
       </c>
       <c r="D313">
-        <f>LEN($E313)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E313" t="s">
@@ -8258,7 +8258,7 @@
         <v>305</v>
       </c>
       <c r="D314">
-        <f>LEN($E314)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E314" t="s">
@@ -8276,7 +8276,7 @@
         <v>306</v>
       </c>
       <c r="D315">
-        <f>LEN($E315)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E315" t="s">
@@ -8294,7 +8294,7 @@
         <v>307</v>
       </c>
       <c r="D316">
-        <f>LEN($E316)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E316" t="s">
@@ -8312,7 +8312,7 @@
         <v>308</v>
       </c>
       <c r="D317">
-        <f>LEN($E317)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E317" t="s">
@@ -8330,7 +8330,7 @@
         <v>309</v>
       </c>
       <c r="D318">
-        <f>LEN($E318)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E318" t="s">
@@ -8348,7 +8348,7 @@
         <v>310</v>
       </c>
       <c r="D319">
-        <f>LEN($E319)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E319" t="s">
@@ -8366,7 +8366,7 @@
         <v>311</v>
       </c>
       <c r="D320">
-        <f>LEN($E320)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E320" t="s">
@@ -8384,7 +8384,7 @@
         <v>312</v>
       </c>
       <c r="D321">
-        <f>LEN($E321)</f>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="E321" t="s">
@@ -8402,7 +8402,7 @@
         <v>313</v>
       </c>
       <c r="D322">
-        <f>LEN($E322)</f>
+        <f t="shared" ref="D322:D387" si="5">LEN($E322)</f>
         <v>266</v>
       </c>
       <c r="E322" t="s">
@@ -8420,7 +8420,7 @@
         <v>314</v>
       </c>
       <c r="D323">
-        <f>LEN($E323)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E323" t="s">
@@ -8438,7 +8438,7 @@
         <v>315</v>
       </c>
       <c r="D324">
-        <f>LEN($E324)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E324" t="s">
@@ -8456,7 +8456,7 @@
         <v>316</v>
       </c>
       <c r="D325">
-        <f>LEN($E325)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E325" t="s">
@@ -8474,7 +8474,7 @@
         <v>317</v>
       </c>
       <c r="D326">
-        <f>LEN($E326)</f>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="E326" t="s">
@@ -8492,7 +8492,7 @@
         <v>318</v>
       </c>
       <c r="D327">
-        <f>LEN($E327)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E327" t="s">
@@ -8510,7 +8510,7 @@
         <v>319</v>
       </c>
       <c r="D328">
-        <f>LEN($E328)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E328" t="s">
@@ -8528,7 +8528,7 @@
         <v>320</v>
       </c>
       <c r="D329">
-        <f>LEN($E329)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E329" t="s">
@@ -8546,7 +8546,7 @@
         <v>321</v>
       </c>
       <c r="D330">
-        <f>LEN($E330)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E330" t="s">
@@ -8564,7 +8564,7 @@
         <v>322</v>
       </c>
       <c r="D331">
-        <f>LEN($E331)</f>
+        <f t="shared" si="5"/>
         <v>358</v>
       </c>
       <c r="E331" t="s">
@@ -8582,7 +8582,7 @@
         <v>323</v>
       </c>
       <c r="D332">
-        <f>LEN($E332)</f>
+        <f t="shared" si="5"/>
         <v>358</v>
       </c>
       <c r="E332" t="s">
@@ -8600,7 +8600,7 @@
         <v>324</v>
       </c>
       <c r="D333">
-        <f>LEN($E333)</f>
+        <f t="shared" si="5"/>
         <v>338</v>
       </c>
       <c r="E333" t="s">
@@ -8618,7 +8618,7 @@
         <v>325</v>
       </c>
       <c r="D334">
-        <f>LEN($E334)</f>
+        <f t="shared" si="5"/>
         <v>338</v>
       </c>
       <c r="E334" t="s">
@@ -8636,7 +8636,7 @@
         <v>326</v>
       </c>
       <c r="D335">
-        <f>LEN($E335)</f>
+        <f t="shared" si="5"/>
         <v>338</v>
       </c>
       <c r="E335" t="s">
@@ -8648,7 +8648,7 @@
         <v>375</v>
       </c>
       <c r="D336">
-        <f>LEN($E336)</f>
+        <f t="shared" si="5"/>
         <v>513</v>
       </c>
       <c r="E336" t="s">
@@ -8663,7 +8663,7 @@
         <v>376</v>
       </c>
       <c r="D337">
-        <f>LEN($E337)</f>
+        <f t="shared" si="5"/>
         <v>327</v>
       </c>
       <c r="E337" t="s">
@@ -8675,7 +8675,7 @@
         <v>377</v>
       </c>
       <c r="D338">
-        <f>LEN($E338)</f>
+        <f t="shared" si="5"/>
         <v>333</v>
       </c>
       <c r="E338" t="s">
@@ -8687,7 +8687,7 @@
         <v>378</v>
       </c>
       <c r="D339">
-        <f>LEN($E339)</f>
+        <f t="shared" si="5"/>
         <v>333</v>
       </c>
       <c r="E339" t="s">
@@ -8702,7 +8702,7 @@
         <v>379</v>
       </c>
       <c r="D340">
-        <f>LEN($E340)</f>
+        <f t="shared" si="5"/>
         <v>335</v>
       </c>
       <c r="E340" t="s">
@@ -8720,7 +8720,7 @@
         <v>380</v>
       </c>
       <c r="D341">
-        <f>LEN($E341)</f>
+        <f t="shared" si="5"/>
         <v>341</v>
       </c>
       <c r="E341" t="s">
@@ -8738,7 +8738,7 @@
         <v>327</v>
       </c>
       <c r="D342">
-        <f>LEN($E342)</f>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="E342" t="s">
@@ -8756,7 +8756,7 @@
         <v>328</v>
       </c>
       <c r="D343">
-        <f>LEN($E343)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E343" t="s">
@@ -8774,7 +8774,7 @@
         <v>329</v>
       </c>
       <c r="D344">
-        <f>LEN($E344)</f>
+        <f t="shared" si="5"/>
         <v>364</v>
       </c>
       <c r="E344" t="s">
@@ -8792,7 +8792,7 @@
         <v>330</v>
       </c>
       <c r="D345">
-        <f>LEN($E345)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E345" t="s">
@@ -8810,7 +8810,7 @@
         <v>331</v>
       </c>
       <c r="D346">
-        <f>LEN($E346)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E346" t="s">
@@ -8828,7 +8828,7 @@
         <v>332</v>
       </c>
       <c r="D347">
-        <f>LEN($E347)</f>
+        <f t="shared" si="5"/>
         <v>357</v>
       </c>
       <c r="E347" t="s">
@@ -8846,7 +8846,7 @@
         <v>333</v>
       </c>
       <c r="D348">
-        <f>LEN($E348)</f>
+        <f t="shared" si="5"/>
         <v>357</v>
       </c>
       <c r="E348" t="s">
@@ -8864,7 +8864,7 @@
         <v>334</v>
       </c>
       <c r="D349">
-        <f>LEN($E349)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E349" t="s">
@@ -8882,7 +8882,7 @@
         <v>335</v>
       </c>
       <c r="D350">
-        <f>LEN($E350)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E350" t="s">
@@ -8900,7 +8900,7 @@
         <v>336</v>
       </c>
       <c r="D351">
-        <f>LEN($E351)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E351" t="s">
@@ -8918,7 +8918,7 @@
         <v>337</v>
       </c>
       <c r="D352">
-        <f>LEN($E352)</f>
+        <f t="shared" si="5"/>
         <v>357</v>
       </c>
       <c r="E352" t="s">
@@ -8936,7 +8936,7 @@
         <v>338</v>
       </c>
       <c r="D353">
-        <f>LEN($E353)</f>
+        <f t="shared" si="5"/>
         <v>365</v>
       </c>
       <c r="E353" t="s">
@@ -8954,7 +8954,7 @@
         <v>339</v>
       </c>
       <c r="D354">
-        <f>LEN($E354)</f>
+        <f t="shared" si="5"/>
         <v>363</v>
       </c>
       <c r="E354" t="s">
@@ -8972,7 +8972,7 @@
         <v>340</v>
       </c>
       <c r="D355">
-        <f>LEN($E355)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E355" t="s">
@@ -8990,7 +8990,7 @@
         <v>341</v>
       </c>
       <c r="D356">
-        <f>LEN($E356)</f>
+        <f t="shared" si="5"/>
         <v>363</v>
       </c>
       <c r="E356" t="s">
@@ -9008,7 +9008,7 @@
         <v>342</v>
       </c>
       <c r="D357">
-        <f>LEN($E357)</f>
+        <f t="shared" si="5"/>
         <v>363</v>
       </c>
       <c r="E357" t="s">
@@ -9026,7 +9026,7 @@
         <v>343</v>
       </c>
       <c r="D358">
-        <f>LEN($E358)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E358" t="s">
@@ -9044,7 +9044,7 @@
         <v>344</v>
       </c>
       <c r="D359">
-        <f>LEN($E359)</f>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="E359" t="s">
@@ -9062,7 +9062,7 @@
         <v>345</v>
       </c>
       <c r="D360">
-        <f>LEN($E360)</f>
+        <f t="shared" si="5"/>
         <v>355</v>
       </c>
       <c r="E360" t="s">
@@ -9080,7 +9080,7 @@
         <v>346</v>
       </c>
       <c r="D361">
-        <f>LEN($E361)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E361" t="s">
@@ -9098,7 +9098,7 @@
         <v>347</v>
       </c>
       <c r="D362">
-        <f>LEN($E362)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E362" t="s">
@@ -9116,7 +9116,7 @@
         <v>348</v>
       </c>
       <c r="D363">
-        <f>LEN($E363)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E363" t="s">
@@ -9134,7 +9134,7 @@
         <v>349</v>
       </c>
       <c r="D364">
-        <f>LEN($E364)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E364" t="s">
@@ -9152,7 +9152,7 @@
         <v>350</v>
       </c>
       <c r="D365">
-        <f>LEN($E365)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E365" t="s">
@@ -9170,7 +9170,7 @@
         <v>351</v>
       </c>
       <c r="D366">
-        <f>LEN($E366)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E366" t="s">
@@ -9188,7 +9188,7 @@
         <v>352</v>
       </c>
       <c r="D367">
-        <f>LEN($E367)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E367" t="s">
@@ -9200,7 +9200,7 @@
         <v>353</v>
       </c>
       <c r="D368">
-        <f>LEN($E368)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9215,7 +9215,7 @@
         <v>354</v>
       </c>
       <c r="D369">
-        <f>LEN($E369)</f>
+        <f t="shared" si="5"/>
         <v>362</v>
       </c>
       <c r="E369" t="s">
@@ -9233,7 +9233,7 @@
         <v>355</v>
       </c>
       <c r="D370">
-        <f>LEN($E370)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E370" t="s">
@@ -9251,7 +9251,7 @@
         <v>356</v>
       </c>
       <c r="D371">
-        <f>LEN($E371)</f>
+        <f t="shared" si="5"/>
         <v>366</v>
       </c>
       <c r="E371" t="s">
@@ -9269,7 +9269,7 @@
         <v>357</v>
       </c>
       <c r="D372">
-        <f>LEN($E372)</f>
+        <f t="shared" si="5"/>
         <v>366</v>
       </c>
       <c r="E372" t="s">
@@ -9287,7 +9287,7 @@
         <v>358</v>
       </c>
       <c r="D373">
-        <f>LEN($E373)</f>
+        <f t="shared" si="5"/>
         <v>366</v>
       </c>
       <c r="E373" t="s">
@@ -9305,7 +9305,7 @@
         <v>359</v>
       </c>
       <c r="D374">
-        <f>LEN($E374)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E374" t="s">
@@ -9323,7 +9323,7 @@
         <v>360</v>
       </c>
       <c r="D375">
-        <f>LEN($E375)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E375" t="s">
@@ -9341,7 +9341,7 @@
         <v>361</v>
       </c>
       <c r="D376">
-        <f>LEN($E376)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E376" t="s">
@@ -9359,7 +9359,7 @@
         <v>362</v>
       </c>
       <c r="D377">
-        <f>LEN($E377)</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="E377" t="s">
@@ -9374,7 +9374,7 @@
         <v>381</v>
       </c>
       <c r="D378">
-        <f>LEN($E378)</f>
+        <f t="shared" si="5"/>
         <v>336</v>
       </c>
       <c r="E378" t="s">
@@ -9392,7 +9392,7 @@
         <v>363</v>
       </c>
       <c r="D379">
-        <f>LEN($E379)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E379" t="s">
@@ -9410,7 +9410,7 @@
         <v>364</v>
       </c>
       <c r="D380">
-        <f>LEN($E380)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E380" t="s">
@@ -9428,7 +9428,7 @@
         <v>365</v>
       </c>
       <c r="D381">
-        <f>LEN($E381)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E381" t="s">
@@ -9446,7 +9446,7 @@
         <v>366</v>
       </c>
       <c r="D382">
-        <f>LEN($E382)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E382" t="s">
@@ -9464,7 +9464,7 @@
         <v>367</v>
       </c>
       <c r="D383">
-        <f>LEN($E383)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E383" t="s">
@@ -9482,7 +9482,7 @@
         <v>368</v>
       </c>
       <c r="D384">
-        <f>LEN($E384)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E384" t="s">
@@ -9500,7 +9500,7 @@
         <v>369</v>
       </c>
       <c r="D385">
-        <f>LEN($E385)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E385" t="s">
@@ -9518,7 +9518,7 @@
         <v>370</v>
       </c>
       <c r="D386">
-        <f>LEN($E386)</f>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="E386" t="s">
@@ -9536,7 +9536,7 @@
         <v>371</v>
       </c>
       <c r="D387">
-        <f>LEN($E387)</f>
+        <f t="shared" si="5"/>
         <v>364</v>
       </c>
       <c r="E387" t="s">

</xml_diff>